<commit_message>
Ahora la variable no se escribe y lee a un excel, además la interfaz gráfica queda en simultaneo con la voz
</commit_message>
<xml_diff>
--- a/Registro.xlsx
+++ b/Registro.xlsx
@@ -439,7 +439,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
@@ -449,7 +449,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Agregado el logo en el video
</commit_message>
<xml_diff>
--- a/Registro.xlsx
+++ b/Registro.xlsx
@@ -449,7 +449,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -459,7 +459,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UI al centro de pantalla
</commit_message>
<xml_diff>
--- a/Registro.xlsx
+++ b/Registro.xlsx
@@ -449,7 +449,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3">
@@ -459,7 +459,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>